<commit_message>
Altered some station codes to be correct
</commit_message>
<xml_diff>
--- a/analysis_2022/data_raw/NCRO_Station_Metadata_CPupd.xlsx
+++ b/analysis_2022/data_raw/NCRO_Station_Metadata_CPupd.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doimspp-my.sharepoint.com/personal/cpien_usbr_gov/Documents/Work/HAB/EDB-HABs-Weeds/analysis_2022/data_raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AE6D83E1-BAF1-48E6-A931-E5ED61DA2D5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{AE6D83E1-BAF1-48E6-A931-E5ED61DA2D5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0FA29982-1BFE-4720-8803-EA780E44FC12}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WQESStation_Metadata_ALL" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="231">
   <si>
     <t>Station</t>
   </si>
@@ -725,9 +725,6 @@
   </si>
   <si>
     <t>NA_RSL</t>
-  </si>
-  <si>
-    <t>NA_INB</t>
   </si>
   <si>
     <t>NA_WER</t>
@@ -1600,8 +1597,8 @@
   <dimension ref="A1:W53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3586,7 +3583,7 @@
         <v>96</v>
       </c>
       <c r="C31" t="s">
-        <v>230</v>
+        <v>97</v>
       </c>
       <c r="D31" t="s">
         <v>87</v>
@@ -4544,7 +4541,7 @@
         <v>85</v>
       </c>
       <c r="C46" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D46" t="s">
         <v>87</v>

</xml_diff>